<commit_message>
criando conteúdo de como criar um repositório, atualizar o README.MD e clonar repositório
</commit_message>
<xml_diff>
--- a/Guithub.xlsx
+++ b/Guithub.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>1 -</t>
   </si>
@@ -182,6 +182,30 @@
   </si>
   <si>
     <t>um novo git status mostrará que o andamento da carga esta ok</t>
+  </si>
+  <si>
+    <t>12 -</t>
+  </si>
+  <si>
+    <t>git commit -m "comente de forma objetiva a atualização do repositório"</t>
+  </si>
+  <si>
+    <t>13 -</t>
+  </si>
+  <si>
+    <t>git status</t>
+  </si>
+  <si>
+    <t>14 -</t>
+  </si>
+  <si>
+    <t>git push origin main fará a carga no repositório</t>
+  </si>
+  <si>
+    <t>15 -</t>
+  </si>
+  <si>
+    <t>F5 mostrará o repositório atualizado</t>
   </si>
 </sst>
 </file>
@@ -1187,6 +1211,193 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>178</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>316057</xdr:colOff>
+      <xdr:row>189</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Imagem 18"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:srcRect r="26858" b="72132"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="542925" y="30299025"/>
+          <a:ext cx="9460057" cy="2038350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>193</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>270712</xdr:colOff>
+      <xdr:row>201</xdr:row>
+      <xdr:rowOff>76019</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Imagem 20"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="542925" y="32870775"/>
+          <a:ext cx="9414712" cy="1447619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>205</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>155864</xdr:colOff>
+      <xdr:row>211</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Imagem 25"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:srcRect t="12761" r="28113" b="71351"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="542925" y="34928175"/>
+          <a:ext cx="9299864" cy="1162050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>215</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>155864</xdr:colOff>
+      <xdr:row>224</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Imagem 27"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:srcRect t="35942" r="28113" b="41920"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="542925" y="36642675"/>
+          <a:ext cx="9299864" cy="1619250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>228</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>94095</xdr:colOff>
+      <xdr:row>259</xdr:row>
+      <xdr:rowOff>18383</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="542925" y="38871525"/>
+          <a:ext cx="9238095" cy="5333333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4151,11 +4362,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:V188"/>
+  <dimension ref="C2:V262"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A158" workbookViewId="0">
-      <selection activeCell="E179" sqref="E179"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8245,29 +8454,1673 @@
       <c r="U186" s="3"/>
       <c r="V186" s="9"/>
     </row>
-    <row r="187" spans="3:22" ht="14.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C187" s="10"/>
-      <c r="D187" s="17"/>
-      <c r="E187" s="11"/>
-      <c r="F187" s="11"/>
-      <c r="G187" s="11"/>
-      <c r="H187" s="11"/>
-      <c r="I187" s="11"/>
-      <c r="J187" s="11"/>
-      <c r="K187" s="11"/>
-      <c r="L187" s="11"/>
-      <c r="M187" s="11"/>
-      <c r="N187" s="11"/>
-      <c r="O187" s="11"/>
-      <c r="P187" s="11"/>
-      <c r="Q187" s="11"/>
-      <c r="R187" s="11"/>
-      <c r="S187" s="11"/>
-      <c r="T187" s="11"/>
-      <c r="U187" s="11"/>
-      <c r="V187" s="12"/>
-    </row>
-    <row r="188" spans="3:22" ht="14.25" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="187" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C187" s="8"/>
+      <c r="D187" s="16"/>
+      <c r="E187" s="3"/>
+      <c r="F187" s="3"/>
+      <c r="G187" s="3"/>
+      <c r="H187" s="3"/>
+      <c r="I187" s="3"/>
+      <c r="J187" s="3"/>
+      <c r="K187" s="3"/>
+      <c r="L187" s="3"/>
+      <c r="M187" s="3"/>
+      <c r="N187" s="3"/>
+      <c r="O187" s="3"/>
+      <c r="P187" s="3"/>
+      <c r="Q187" s="3"/>
+      <c r="R187" s="3"/>
+      <c r="S187" s="3"/>
+      <c r="T187" s="3"/>
+      <c r="U187" s="3"/>
+      <c r="V187" s="9"/>
+    </row>
+    <row r="188" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C188" s="8"/>
+      <c r="D188" s="16"/>
+      <c r="E188" s="3"/>
+      <c r="F188" s="3"/>
+      <c r="G188" s="3"/>
+      <c r="H188" s="3"/>
+      <c r="I188" s="3"/>
+      <c r="J188" s="3"/>
+      <c r="K188" s="3"/>
+      <c r="L188" s="3"/>
+      <c r="M188" s="3"/>
+      <c r="N188" s="3"/>
+      <c r="O188" s="3"/>
+      <c r="P188" s="3"/>
+      <c r="Q188" s="3"/>
+      <c r="R188" s="3"/>
+      <c r="S188" s="3"/>
+      <c r="T188" s="3"/>
+      <c r="U188" s="3"/>
+      <c r="V188" s="9"/>
+    </row>
+    <row r="189" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C189" s="8"/>
+      <c r="D189" s="16"/>
+      <c r="E189" s="3"/>
+      <c r="F189" s="3"/>
+      <c r="G189" s="3"/>
+      <c r="H189" s="3"/>
+      <c r="I189" s="3"/>
+      <c r="J189" s="3"/>
+      <c r="K189" s="3"/>
+      <c r="L189" s="3"/>
+      <c r="M189" s="3"/>
+      <c r="N189" s="3"/>
+      <c r="O189" s="3"/>
+      <c r="P189" s="3"/>
+      <c r="Q189" s="3"/>
+      <c r="R189" s="3"/>
+      <c r="S189" s="3"/>
+      <c r="T189" s="3"/>
+      <c r="U189" s="3"/>
+      <c r="V189" s="9"/>
+    </row>
+    <row r="190" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C190" s="8"/>
+      <c r="D190" s="16"/>
+      <c r="E190" s="3"/>
+      <c r="F190" s="3"/>
+      <c r="G190" s="3"/>
+      <c r="H190" s="3"/>
+      <c r="I190" s="3"/>
+      <c r="J190" s="3"/>
+      <c r="K190" s="3"/>
+      <c r="L190" s="3"/>
+      <c r="M190" s="3"/>
+      <c r="N190" s="3"/>
+      <c r="O190" s="3"/>
+      <c r="P190" s="3"/>
+      <c r="Q190" s="3"/>
+      <c r="R190" s="3"/>
+      <c r="S190" s="3"/>
+      <c r="T190" s="3"/>
+      <c r="U190" s="3"/>
+      <c r="V190" s="9"/>
+    </row>
+    <row r="191" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C191" s="8"/>
+      <c r="D191" s="16"/>
+      <c r="E191" s="3"/>
+      <c r="F191" s="3"/>
+      <c r="G191" s="3"/>
+      <c r="H191" s="3"/>
+      <c r="I191" s="3"/>
+      <c r="J191" s="3"/>
+      <c r="K191" s="3"/>
+      <c r="L191" s="3"/>
+      <c r="M191" s="3"/>
+      <c r="N191" s="3"/>
+      <c r="O191" s="3"/>
+      <c r="P191" s="3"/>
+      <c r="Q191" s="3"/>
+      <c r="R191" s="3"/>
+      <c r="S191" s="3"/>
+      <c r="T191" s="3"/>
+      <c r="U191" s="3"/>
+      <c r="V191" s="9"/>
+    </row>
+    <row r="192" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C192" s="8"/>
+      <c r="D192" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E192" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F192" s="3"/>
+      <c r="G192" s="3"/>
+      <c r="H192" s="3"/>
+      <c r="I192" s="3"/>
+      <c r="J192" s="3"/>
+      <c r="K192" s="3"/>
+      <c r="L192" s="3"/>
+      <c r="M192" s="3"/>
+      <c r="N192" s="3"/>
+      <c r="O192" s="3"/>
+      <c r="P192" s="3"/>
+      <c r="Q192" s="3"/>
+      <c r="R192" s="3"/>
+      <c r="S192" s="3"/>
+      <c r="T192" s="3"/>
+      <c r="U192" s="3"/>
+      <c r="V192" s="9"/>
+    </row>
+    <row r="193" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C193" s="8"/>
+      <c r="D193" s="16"/>
+      <c r="E193" s="3"/>
+      <c r="F193" s="3"/>
+      <c r="G193" s="3"/>
+      <c r="H193" s="3"/>
+      <c r="I193" s="3"/>
+      <c r="J193" s="3"/>
+      <c r="K193" s="3"/>
+      <c r="L193" s="3"/>
+      <c r="M193" s="3"/>
+      <c r="N193" s="3"/>
+      <c r="O193" s="3"/>
+      <c r="P193" s="3"/>
+      <c r="Q193" s="3"/>
+      <c r="R193" s="3"/>
+      <c r="S193" s="3"/>
+      <c r="T193" s="3"/>
+      <c r="U193" s="3"/>
+      <c r="V193" s="9"/>
+    </row>
+    <row r="194" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C194" s="8"/>
+      <c r="D194" s="16"/>
+      <c r="E194" s="3"/>
+      <c r="F194" s="3"/>
+      <c r="G194" s="3"/>
+      <c r="H194" s="3"/>
+      <c r="I194" s="3"/>
+      <c r="J194" s="3"/>
+      <c r="K194" s="3"/>
+      <c r="L194" s="3"/>
+      <c r="M194" s="3"/>
+      <c r="N194" s="3"/>
+      <c r="O194" s="3"/>
+      <c r="P194" s="3"/>
+      <c r="Q194" s="3"/>
+      <c r="R194" s="3"/>
+      <c r="S194" s="3"/>
+      <c r="T194" s="3"/>
+      <c r="U194" s="3"/>
+      <c r="V194" s="9"/>
+    </row>
+    <row r="195" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C195" s="8"/>
+      <c r="D195" s="16"/>
+      <c r="E195" s="3"/>
+      <c r="F195" s="3"/>
+      <c r="G195" s="3"/>
+      <c r="H195" s="3"/>
+      <c r="I195" s="3"/>
+      <c r="J195" s="3"/>
+      <c r="K195" s="3"/>
+      <c r="L195" s="3"/>
+      <c r="M195" s="3"/>
+      <c r="N195" s="3"/>
+      <c r="O195" s="3"/>
+      <c r="P195" s="3"/>
+      <c r="Q195" s="3"/>
+      <c r="R195" s="3"/>
+      <c r="S195" s="3"/>
+      <c r="T195" s="3"/>
+      <c r="U195" s="3"/>
+      <c r="V195" s="9"/>
+    </row>
+    <row r="196" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C196" s="8"/>
+      <c r="D196" s="16"/>
+      <c r="E196" s="3"/>
+      <c r="F196" s="3"/>
+      <c r="G196" s="3"/>
+      <c r="H196" s="3"/>
+      <c r="I196" s="3"/>
+      <c r="J196" s="3"/>
+      <c r="K196" s="3"/>
+      <c r="L196" s="3"/>
+      <c r="M196" s="3"/>
+      <c r="N196" s="3"/>
+      <c r="O196" s="3"/>
+      <c r="P196" s="3"/>
+      <c r="Q196" s="3"/>
+      <c r="R196" s="3"/>
+      <c r="S196" s="3"/>
+      <c r="T196" s="3"/>
+      <c r="U196" s="3"/>
+      <c r="V196" s="9"/>
+    </row>
+    <row r="197" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C197" s="8"/>
+      <c r="D197" s="16"/>
+      <c r="E197" s="3"/>
+      <c r="F197" s="3"/>
+      <c r="G197" s="3"/>
+      <c r="H197" s="3"/>
+      <c r="I197" s="3"/>
+      <c r="J197" s="3"/>
+      <c r="K197" s="3"/>
+      <c r="L197" s="3"/>
+      <c r="M197" s="3"/>
+      <c r="N197" s="3"/>
+      <c r="O197" s="3"/>
+      <c r="P197" s="3"/>
+      <c r="Q197" s="3"/>
+      <c r="R197" s="3"/>
+      <c r="S197" s="3"/>
+      <c r="T197" s="3"/>
+      <c r="U197" s="3"/>
+      <c r="V197" s="9"/>
+    </row>
+    <row r="198" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C198" s="8"/>
+      <c r="D198" s="16"/>
+      <c r="E198" s="3"/>
+      <c r="F198" s="3"/>
+      <c r="G198" s="3"/>
+      <c r="H198" s="3"/>
+      <c r="I198" s="3"/>
+      <c r="J198" s="3"/>
+      <c r="K198" s="3"/>
+      <c r="L198" s="3"/>
+      <c r="M198" s="3"/>
+      <c r="N198" s="3"/>
+      <c r="O198" s="3"/>
+      <c r="P198" s="3"/>
+      <c r="Q198" s="3"/>
+      <c r="R198" s="3"/>
+      <c r="S198" s="3"/>
+      <c r="T198" s="3"/>
+      <c r="U198" s="3"/>
+      <c r="V198" s="9"/>
+    </row>
+    <row r="199" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C199" s="8"/>
+      <c r="D199" s="16"/>
+      <c r="E199" s="3"/>
+      <c r="F199" s="3"/>
+      <c r="G199" s="3"/>
+      <c r="H199" s="3"/>
+      <c r="I199" s="3"/>
+      <c r="J199" s="3"/>
+      <c r="K199" s="3"/>
+      <c r="L199" s="3"/>
+      <c r="M199" s="3"/>
+      <c r="N199" s="3"/>
+      <c r="O199" s="3"/>
+      <c r="P199" s="3"/>
+      <c r="Q199" s="3"/>
+      <c r="R199" s="3"/>
+      <c r="S199" s="3"/>
+      <c r="T199" s="3"/>
+      <c r="U199" s="3"/>
+      <c r="V199" s="9"/>
+    </row>
+    <row r="200" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C200" s="8"/>
+      <c r="D200" s="16"/>
+      <c r="E200" s="3"/>
+      <c r="F200" s="3"/>
+      <c r="G200" s="3"/>
+      <c r="H200" s="3"/>
+      <c r="I200" s="3"/>
+      <c r="J200" s="3"/>
+      <c r="K200" s="3"/>
+      <c r="L200" s="3"/>
+      <c r="M200" s="3"/>
+      <c r="N200" s="3"/>
+      <c r="O200" s="3"/>
+      <c r="P200" s="3"/>
+      <c r="Q200" s="3"/>
+      <c r="R200" s="3"/>
+      <c r="S200" s="3"/>
+      <c r="T200" s="3"/>
+      <c r="U200" s="3"/>
+      <c r="V200" s="9"/>
+    </row>
+    <row r="201" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C201" s="8"/>
+      <c r="D201" s="16"/>
+      <c r="E201" s="3"/>
+      <c r="F201" s="3"/>
+      <c r="G201" s="3"/>
+      <c r="H201" s="3"/>
+      <c r="I201" s="3"/>
+      <c r="J201" s="3"/>
+      <c r="K201" s="3"/>
+      <c r="L201" s="3"/>
+      <c r="M201" s="3"/>
+      <c r="N201" s="3"/>
+      <c r="O201" s="3"/>
+      <c r="P201" s="3"/>
+      <c r="Q201" s="3"/>
+      <c r="R201" s="3"/>
+      <c r="S201" s="3"/>
+      <c r="T201" s="3"/>
+      <c r="U201" s="3"/>
+      <c r="V201" s="9"/>
+    </row>
+    <row r="202" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C202" s="8"/>
+      <c r="D202" s="16"/>
+      <c r="E202" s="3"/>
+      <c r="F202" s="3"/>
+      <c r="G202" s="3"/>
+      <c r="H202" s="3"/>
+      <c r="I202" s="3"/>
+      <c r="J202" s="3"/>
+      <c r="K202" s="3"/>
+      <c r="L202" s="3"/>
+      <c r="M202" s="3"/>
+      <c r="N202" s="3"/>
+      <c r="O202" s="3"/>
+      <c r="P202" s="3"/>
+      <c r="Q202" s="3"/>
+      <c r="R202" s="3"/>
+      <c r="S202" s="3"/>
+      <c r="T202" s="3"/>
+      <c r="U202" s="3"/>
+      <c r="V202" s="9"/>
+    </row>
+    <row r="203" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C203" s="8"/>
+      <c r="D203" s="16"/>
+      <c r="E203" s="3"/>
+      <c r="F203" s="3"/>
+      <c r="G203" s="3"/>
+      <c r="H203" s="3"/>
+      <c r="I203" s="3"/>
+      <c r="J203" s="3"/>
+      <c r="K203" s="3"/>
+      <c r="L203" s="3"/>
+      <c r="M203" s="3"/>
+      <c r="N203" s="3"/>
+      <c r="O203" s="3"/>
+      <c r="P203" s="3"/>
+      <c r="Q203" s="3"/>
+      <c r="R203" s="3"/>
+      <c r="S203" s="3"/>
+      <c r="T203" s="3"/>
+      <c r="U203" s="3"/>
+      <c r="V203" s="9"/>
+    </row>
+    <row r="204" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C204" s="8"/>
+      <c r="D204" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E204" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F204" s="3"/>
+      <c r="G204" s="3"/>
+      <c r="H204" s="3"/>
+      <c r="I204" s="3"/>
+      <c r="J204" s="3"/>
+      <c r="K204" s="3"/>
+      <c r="L204" s="3"/>
+      <c r="M204" s="3"/>
+      <c r="N204" s="3"/>
+      <c r="O204" s="3"/>
+      <c r="P204" s="3"/>
+      <c r="Q204" s="3"/>
+      <c r="R204" s="3"/>
+      <c r="S204" s="3"/>
+      <c r="T204" s="3"/>
+      <c r="U204" s="3"/>
+      <c r="V204" s="9"/>
+    </row>
+    <row r="205" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C205" s="8"/>
+      <c r="D205" s="16"/>
+      <c r="E205" s="3"/>
+      <c r="F205" s="3"/>
+      <c r="G205" s="3"/>
+      <c r="H205" s="3"/>
+      <c r="I205" s="3"/>
+      <c r="J205" s="3"/>
+      <c r="K205" s="3"/>
+      <c r="L205" s="3"/>
+      <c r="M205" s="3"/>
+      <c r="N205" s="3"/>
+      <c r="O205" s="3"/>
+      <c r="P205" s="3"/>
+      <c r="Q205" s="3"/>
+      <c r="R205" s="3"/>
+      <c r="S205" s="3"/>
+      <c r="T205" s="3"/>
+      <c r="U205" s="3"/>
+      <c r="V205" s="9"/>
+    </row>
+    <row r="206" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C206" s="8"/>
+      <c r="D206" s="16"/>
+      <c r="E206" s="3"/>
+      <c r="F206" s="3"/>
+      <c r="G206" s="3"/>
+      <c r="H206" s="3"/>
+      <c r="I206" s="3"/>
+      <c r="J206" s="3"/>
+      <c r="K206" s="3"/>
+      <c r="L206" s="3"/>
+      <c r="M206" s="3"/>
+      <c r="N206" s="3"/>
+      <c r="O206" s="3"/>
+      <c r="P206" s="3"/>
+      <c r="Q206" s="3"/>
+      <c r="R206" s="3"/>
+      <c r="S206" s="3"/>
+      <c r="T206" s="3"/>
+      <c r="U206" s="3"/>
+      <c r="V206" s="9"/>
+    </row>
+    <row r="207" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C207" s="8"/>
+      <c r="D207" s="16"/>
+      <c r="E207" s="3"/>
+      <c r="F207" s="3"/>
+      <c r="G207" s="3"/>
+      <c r="H207" s="3"/>
+      <c r="I207" s="3"/>
+      <c r="J207" s="3"/>
+      <c r="K207" s="3"/>
+      <c r="L207" s="3"/>
+      <c r="M207" s="3"/>
+      <c r="N207" s="3"/>
+      <c r="O207" s="3"/>
+      <c r="P207" s="3"/>
+      <c r="Q207" s="3"/>
+      <c r="R207" s="3"/>
+      <c r="S207" s="3"/>
+      <c r="T207" s="3"/>
+      <c r="U207" s="3"/>
+      <c r="V207" s="9"/>
+    </row>
+    <row r="208" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C208" s="8"/>
+      <c r="D208" s="16"/>
+      <c r="E208" s="3"/>
+      <c r="F208" s="3"/>
+      <c r="G208" s="3"/>
+      <c r="H208" s="3"/>
+      <c r="I208" s="3"/>
+      <c r="J208" s="3"/>
+      <c r="K208" s="3"/>
+      <c r="L208" s="3"/>
+      <c r="M208" s="3"/>
+      <c r="N208" s="3"/>
+      <c r="O208" s="3"/>
+      <c r="P208" s="3"/>
+      <c r="Q208" s="3"/>
+      <c r="R208" s="3"/>
+      <c r="S208" s="3"/>
+      <c r="T208" s="3"/>
+      <c r="U208" s="3"/>
+      <c r="V208" s="9"/>
+    </row>
+    <row r="209" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C209" s="8"/>
+      <c r="D209" s="16"/>
+      <c r="E209" s="3"/>
+      <c r="F209" s="3"/>
+      <c r="G209" s="3"/>
+      <c r="H209" s="3"/>
+      <c r="I209" s="3"/>
+      <c r="J209" s="3"/>
+      <c r="K209" s="3"/>
+      <c r="L209" s="3"/>
+      <c r="M209" s="3"/>
+      <c r="N209" s="3"/>
+      <c r="O209" s="3"/>
+      <c r="P209" s="3"/>
+      <c r="Q209" s="3"/>
+      <c r="R209" s="3"/>
+      <c r="S209" s="3"/>
+      <c r="T209" s="3"/>
+      <c r="U209" s="3"/>
+      <c r="V209" s="9"/>
+    </row>
+    <row r="210" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C210" s="8"/>
+      <c r="D210" s="16"/>
+      <c r="E210" s="3"/>
+      <c r="F210" s="3"/>
+      <c r="G210" s="3"/>
+      <c r="H210" s="3"/>
+      <c r="I210" s="3"/>
+      <c r="J210" s="3"/>
+      <c r="K210" s="3"/>
+      <c r="L210" s="3"/>
+      <c r="M210" s="3"/>
+      <c r="N210" s="3"/>
+      <c r="O210" s="3"/>
+      <c r="P210" s="3"/>
+      <c r="Q210" s="3"/>
+      <c r="R210" s="3"/>
+      <c r="S210" s="3"/>
+      <c r="T210" s="3"/>
+      <c r="U210" s="3"/>
+      <c r="V210" s="9"/>
+    </row>
+    <row r="211" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C211" s="8"/>
+      <c r="D211" s="16"/>
+      <c r="E211" s="3"/>
+      <c r="F211" s="3"/>
+      <c r="G211" s="3"/>
+      <c r="H211" s="3"/>
+      <c r="I211" s="3"/>
+      <c r="J211" s="3"/>
+      <c r="K211" s="3"/>
+      <c r="L211" s="3"/>
+      <c r="M211" s="3"/>
+      <c r="N211" s="3"/>
+      <c r="O211" s="3"/>
+      <c r="P211" s="3"/>
+      <c r="Q211" s="3"/>
+      <c r="R211" s="3"/>
+      <c r="S211" s="3"/>
+      <c r="T211" s="3"/>
+      <c r="U211" s="3"/>
+      <c r="V211" s="9"/>
+    </row>
+    <row r="212" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C212" s="8"/>
+      <c r="D212" s="16"/>
+      <c r="E212" s="3"/>
+      <c r="F212" s="3"/>
+      <c r="G212" s="3"/>
+      <c r="H212" s="3"/>
+      <c r="I212" s="3"/>
+      <c r="J212" s="3"/>
+      <c r="K212" s="3"/>
+      <c r="L212" s="3"/>
+      <c r="M212" s="3"/>
+      <c r="N212" s="3"/>
+      <c r="O212" s="3"/>
+      <c r="P212" s="3"/>
+      <c r="Q212" s="3"/>
+      <c r="R212" s="3"/>
+      <c r="S212" s="3"/>
+      <c r="T212" s="3"/>
+      <c r="U212" s="3"/>
+      <c r="V212" s="9"/>
+    </row>
+    <row r="213" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C213" s="8"/>
+      <c r="D213" s="16"/>
+      <c r="E213" s="3"/>
+      <c r="F213" s="3"/>
+      <c r="G213" s="3"/>
+      <c r="H213" s="3"/>
+      <c r="I213" s="3"/>
+      <c r="J213" s="3"/>
+      <c r="K213" s="3"/>
+      <c r="L213" s="3"/>
+      <c r="M213" s="3"/>
+      <c r="N213" s="3"/>
+      <c r="O213" s="3"/>
+      <c r="P213" s="3"/>
+      <c r="Q213" s="3"/>
+      <c r="R213" s="3"/>
+      <c r="S213" s="3"/>
+      <c r="T213" s="3"/>
+      <c r="U213" s="3"/>
+      <c r="V213" s="9"/>
+    </row>
+    <row r="214" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C214" s="8"/>
+      <c r="D214" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E214" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F214" s="3"/>
+      <c r="G214" s="3"/>
+      <c r="H214" s="3"/>
+      <c r="I214" s="3"/>
+      <c r="J214" s="3"/>
+      <c r="K214" s="3"/>
+      <c r="L214" s="3"/>
+      <c r="M214" s="3"/>
+      <c r="N214" s="3"/>
+      <c r="O214" s="3"/>
+      <c r="P214" s="3"/>
+      <c r="Q214" s="3"/>
+      <c r="R214" s="3"/>
+      <c r="S214" s="3"/>
+      <c r="T214" s="3"/>
+      <c r="U214" s="3"/>
+      <c r="V214" s="9"/>
+    </row>
+    <row r="215" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C215" s="8"/>
+      <c r="D215" s="16"/>
+      <c r="E215" s="3"/>
+      <c r="F215" s="3"/>
+      <c r="G215" s="3"/>
+      <c r="H215" s="3"/>
+      <c r="I215" s="3"/>
+      <c r="J215" s="3"/>
+      <c r="K215" s="3"/>
+      <c r="L215" s="3"/>
+      <c r="M215" s="3"/>
+      <c r="N215" s="3"/>
+      <c r="O215" s="3"/>
+      <c r="P215" s="3"/>
+      <c r="Q215" s="3"/>
+      <c r="R215" s="3"/>
+      <c r="S215" s="3"/>
+      <c r="T215" s="3"/>
+      <c r="U215" s="3"/>
+      <c r="V215" s="9"/>
+    </row>
+    <row r="216" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C216" s="8"/>
+      <c r="D216" s="16"/>
+      <c r="E216" s="3"/>
+      <c r="F216" s="3"/>
+      <c r="G216" s="3"/>
+      <c r="H216" s="3"/>
+      <c r="I216" s="3"/>
+      <c r="J216" s="3"/>
+      <c r="K216" s="3"/>
+      <c r="L216" s="3"/>
+      <c r="M216" s="3"/>
+      <c r="N216" s="3"/>
+      <c r="O216" s="3"/>
+      <c r="P216" s="3"/>
+      <c r="Q216" s="3"/>
+      <c r="R216" s="3"/>
+      <c r="S216" s="3"/>
+      <c r="T216" s="3"/>
+      <c r="U216" s="3"/>
+      <c r="V216" s="9"/>
+    </row>
+    <row r="217" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C217" s="8"/>
+      <c r="D217" s="16"/>
+      <c r="E217" s="3"/>
+      <c r="F217" s="3"/>
+      <c r="G217" s="3"/>
+      <c r="H217" s="3"/>
+      <c r="I217" s="3"/>
+      <c r="J217" s="3"/>
+      <c r="K217" s="3"/>
+      <c r="L217" s="3"/>
+      <c r="M217" s="3"/>
+      <c r="N217" s="3"/>
+      <c r="O217" s="3"/>
+      <c r="P217" s="3"/>
+      <c r="Q217" s="3"/>
+      <c r="R217" s="3"/>
+      <c r="S217" s="3"/>
+      <c r="T217" s="3"/>
+      <c r="U217" s="3"/>
+      <c r="V217" s="9"/>
+    </row>
+    <row r="218" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C218" s="8"/>
+      <c r="D218" s="16"/>
+      <c r="E218" s="3"/>
+      <c r="F218" s="3"/>
+      <c r="G218" s="3"/>
+      <c r="H218" s="3"/>
+      <c r="I218" s="3"/>
+      <c r="J218" s="3"/>
+      <c r="K218" s="3"/>
+      <c r="L218" s="3"/>
+      <c r="M218" s="3"/>
+      <c r="N218" s="3"/>
+      <c r="O218" s="3"/>
+      <c r="P218" s="3"/>
+      <c r="Q218" s="3"/>
+      <c r="R218" s="3"/>
+      <c r="S218" s="3"/>
+      <c r="T218" s="3"/>
+      <c r="U218" s="3"/>
+      <c r="V218" s="9"/>
+    </row>
+    <row r="219" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C219" s="8"/>
+      <c r="D219" s="16"/>
+      <c r="E219" s="3"/>
+      <c r="F219" s="3"/>
+      <c r="G219" s="3"/>
+      <c r="H219" s="3"/>
+      <c r="I219" s="3"/>
+      <c r="J219" s="3"/>
+      <c r="K219" s="3"/>
+      <c r="L219" s="3"/>
+      <c r="M219" s="3"/>
+      <c r="N219" s="3"/>
+      <c r="O219" s="3"/>
+      <c r="P219" s="3"/>
+      <c r="Q219" s="3"/>
+      <c r="R219" s="3"/>
+      <c r="S219" s="3"/>
+      <c r="T219" s="3"/>
+      <c r="U219" s="3"/>
+      <c r="V219" s="9"/>
+    </row>
+    <row r="220" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C220" s="8"/>
+      <c r="D220" s="16"/>
+      <c r="E220" s="3"/>
+      <c r="F220" s="3"/>
+      <c r="G220" s="3"/>
+      <c r="H220" s="3"/>
+      <c r="I220" s="3"/>
+      <c r="J220" s="3"/>
+      <c r="K220" s="3"/>
+      <c r="L220" s="3"/>
+      <c r="M220" s="3"/>
+      <c r="N220" s="3"/>
+      <c r="O220" s="3"/>
+      <c r="P220" s="3"/>
+      <c r="Q220" s="3"/>
+      <c r="R220" s="3"/>
+      <c r="S220" s="3"/>
+      <c r="T220" s="3"/>
+      <c r="U220" s="3"/>
+      <c r="V220" s="9"/>
+    </row>
+    <row r="221" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C221" s="8"/>
+      <c r="D221" s="16"/>
+      <c r="E221" s="3"/>
+      <c r="F221" s="3"/>
+      <c r="G221" s="3"/>
+      <c r="H221" s="3"/>
+      <c r="I221" s="3"/>
+      <c r="J221" s="3"/>
+      <c r="K221" s="3"/>
+      <c r="L221" s="3"/>
+      <c r="M221" s="3"/>
+      <c r="N221" s="3"/>
+      <c r="O221" s="3"/>
+      <c r="P221" s="3"/>
+      <c r="Q221" s="3"/>
+      <c r="R221" s="3"/>
+      <c r="S221" s="3"/>
+      <c r="T221" s="3"/>
+      <c r="U221" s="3"/>
+      <c r="V221" s="9"/>
+    </row>
+    <row r="222" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C222" s="8"/>
+      <c r="D222" s="16"/>
+      <c r="E222" s="3"/>
+      <c r="F222" s="3"/>
+      <c r="G222" s="3"/>
+      <c r="H222" s="3"/>
+      <c r="I222" s="3"/>
+      <c r="J222" s="3"/>
+      <c r="K222" s="3"/>
+      <c r="L222" s="3"/>
+      <c r="M222" s="3"/>
+      <c r="N222" s="3"/>
+      <c r="O222" s="3"/>
+      <c r="P222" s="3"/>
+      <c r="Q222" s="3"/>
+      <c r="R222" s="3"/>
+      <c r="S222" s="3"/>
+      <c r="T222" s="3"/>
+      <c r="U222" s="3"/>
+      <c r="V222" s="9"/>
+    </row>
+    <row r="223" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C223" s="8"/>
+      <c r="D223" s="16"/>
+      <c r="E223" s="3"/>
+      <c r="F223" s="3"/>
+      <c r="G223" s="3"/>
+      <c r="H223" s="3"/>
+      <c r="I223" s="3"/>
+      <c r="J223" s="3"/>
+      <c r="K223" s="3"/>
+      <c r="L223" s="3"/>
+      <c r="M223" s="3"/>
+      <c r="N223" s="3"/>
+      <c r="O223" s="3"/>
+      <c r="P223" s="3"/>
+      <c r="Q223" s="3"/>
+      <c r="R223" s="3"/>
+      <c r="S223" s="3"/>
+      <c r="T223" s="3"/>
+      <c r="U223" s="3"/>
+      <c r="V223" s="9"/>
+    </row>
+    <row r="224" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C224" s="8"/>
+      <c r="D224" s="16"/>
+      <c r="E224" s="3"/>
+      <c r="F224" s="3"/>
+      <c r="G224" s="3"/>
+      <c r="H224" s="3"/>
+      <c r="I224" s="3"/>
+      <c r="J224" s="3"/>
+      <c r="K224" s="3"/>
+      <c r="L224" s="3"/>
+      <c r="M224" s="3"/>
+      <c r="N224" s="3"/>
+      <c r="O224" s="3"/>
+      <c r="P224" s="3"/>
+      <c r="Q224" s="3"/>
+      <c r="R224" s="3"/>
+      <c r="S224" s="3"/>
+      <c r="T224" s="3"/>
+      <c r="U224" s="3"/>
+      <c r="V224" s="9"/>
+    </row>
+    <row r="225" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C225" s="8"/>
+      <c r="D225" s="16"/>
+      <c r="E225" s="3"/>
+      <c r="F225" s="3"/>
+      <c r="G225" s="3"/>
+      <c r="H225" s="3"/>
+      <c r="I225" s="3"/>
+      <c r="J225" s="3"/>
+      <c r="K225" s="3"/>
+      <c r="L225" s="3"/>
+      <c r="M225" s="3"/>
+      <c r="N225" s="3"/>
+      <c r="O225" s="3"/>
+      <c r="P225" s="3"/>
+      <c r="Q225" s="3"/>
+      <c r="R225" s="3"/>
+      <c r="S225" s="3"/>
+      <c r="T225" s="3"/>
+      <c r="U225" s="3"/>
+      <c r="V225" s="9"/>
+    </row>
+    <row r="226" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C226" s="8"/>
+      <c r="D226" s="16"/>
+      <c r="E226" s="3"/>
+      <c r="F226" s="3"/>
+      <c r="G226" s="3"/>
+      <c r="H226" s="3"/>
+      <c r="I226" s="3"/>
+      <c r="J226" s="3"/>
+      <c r="K226" s="3"/>
+      <c r="L226" s="3"/>
+      <c r="M226" s="3"/>
+      <c r="N226" s="3"/>
+      <c r="O226" s="3"/>
+      <c r="P226" s="3"/>
+      <c r="Q226" s="3"/>
+      <c r="R226" s="3"/>
+      <c r="S226" s="3"/>
+      <c r="T226" s="3"/>
+      <c r="U226" s="3"/>
+      <c r="V226" s="9"/>
+    </row>
+    <row r="227" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C227" s="8"/>
+      <c r="D227" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E227" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F227" s="3"/>
+      <c r="G227" s="3"/>
+      <c r="H227" s="3"/>
+      <c r="I227" s="3"/>
+      <c r="J227" s="3"/>
+      <c r="K227" s="3"/>
+      <c r="L227" s="3"/>
+      <c r="M227" s="3"/>
+      <c r="N227" s="3"/>
+      <c r="O227" s="3"/>
+      <c r="P227" s="3"/>
+      <c r="Q227" s="3"/>
+      <c r="R227" s="3"/>
+      <c r="S227" s="3"/>
+      <c r="T227" s="3"/>
+      <c r="U227" s="3"/>
+      <c r="V227" s="9"/>
+    </row>
+    <row r="228" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C228" s="8"/>
+      <c r="D228" s="16"/>
+      <c r="E228" s="3"/>
+      <c r="F228" s="3"/>
+      <c r="G228" s="3"/>
+      <c r="H228" s="3"/>
+      <c r="I228" s="3"/>
+      <c r="J228" s="3"/>
+      <c r="K228" s="3"/>
+      <c r="L228" s="3"/>
+      <c r="M228" s="3"/>
+      <c r="N228" s="3"/>
+      <c r="O228" s="3"/>
+      <c r="P228" s="3"/>
+      <c r="Q228" s="3"/>
+      <c r="R228" s="3"/>
+      <c r="S228" s="3"/>
+      <c r="T228" s="3"/>
+      <c r="U228" s="3"/>
+      <c r="V228" s="9"/>
+    </row>
+    <row r="229" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C229" s="8"/>
+      <c r="D229" s="16"/>
+      <c r="E229" s="3"/>
+      <c r="F229" s="3"/>
+      <c r="G229" s="3"/>
+      <c r="H229" s="3"/>
+      <c r="I229" s="3"/>
+      <c r="J229" s="3"/>
+      <c r="K229" s="3"/>
+      <c r="L229" s="3"/>
+      <c r="M229" s="3"/>
+      <c r="N229" s="3"/>
+      <c r="O229" s="3"/>
+      <c r="P229" s="3"/>
+      <c r="Q229" s="3"/>
+      <c r="R229" s="3"/>
+      <c r="S229" s="3"/>
+      <c r="T229" s="3"/>
+      <c r="U229" s="3"/>
+      <c r="V229" s="9"/>
+    </row>
+    <row r="230" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C230" s="8"/>
+      <c r="D230" s="16"/>
+      <c r="E230" s="3"/>
+      <c r="F230" s="3"/>
+      <c r="G230" s="3"/>
+      <c r="H230" s="3"/>
+      <c r="I230" s="3"/>
+      <c r="J230" s="3"/>
+      <c r="K230" s="3"/>
+      <c r="L230" s="3"/>
+      <c r="M230" s="3"/>
+      <c r="N230" s="3"/>
+      <c r="O230" s="3"/>
+      <c r="P230" s="3"/>
+      <c r="Q230" s="3"/>
+      <c r="R230" s="3"/>
+      <c r="S230" s="3"/>
+      <c r="T230" s="3"/>
+      <c r="U230" s="3"/>
+      <c r="V230" s="9"/>
+    </row>
+    <row r="231" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C231" s="8"/>
+      <c r="D231" s="16"/>
+      <c r="E231" s="3"/>
+      <c r="F231" s="3"/>
+      <c r="G231" s="3"/>
+      <c r="H231" s="3"/>
+      <c r="I231" s="3"/>
+      <c r="J231" s="3"/>
+      <c r="K231" s="3"/>
+      <c r="L231" s="3"/>
+      <c r="M231" s="3"/>
+      <c r="N231" s="3"/>
+      <c r="O231" s="3"/>
+      <c r="P231" s="3"/>
+      <c r="Q231" s="3"/>
+      <c r="R231" s="3"/>
+      <c r="S231" s="3"/>
+      <c r="T231" s="3"/>
+      <c r="U231" s="3"/>
+      <c r="V231" s="9"/>
+    </row>
+    <row r="232" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C232" s="8"/>
+      <c r="D232" s="16"/>
+      <c r="E232" s="3"/>
+      <c r="F232" s="3"/>
+      <c r="G232" s="3"/>
+      <c r="H232" s="3"/>
+      <c r="I232" s="3"/>
+      <c r="J232" s="3"/>
+      <c r="K232" s="3"/>
+      <c r="L232" s="3"/>
+      <c r="M232" s="3"/>
+      <c r="N232" s="3"/>
+      <c r="O232" s="3"/>
+      <c r="P232" s="3"/>
+      <c r="Q232" s="3"/>
+      <c r="R232" s="3"/>
+      <c r="S232" s="3"/>
+      <c r="T232" s="3"/>
+      <c r="U232" s="3"/>
+      <c r="V232" s="9"/>
+    </row>
+    <row r="233" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C233" s="8"/>
+      <c r="D233" s="16"/>
+      <c r="E233" s="3"/>
+      <c r="F233" s="3"/>
+      <c r="G233" s="3"/>
+      <c r="H233" s="3"/>
+      <c r="I233" s="3"/>
+      <c r="J233" s="3"/>
+      <c r="K233" s="3"/>
+      <c r="L233" s="3"/>
+      <c r="M233" s="3"/>
+      <c r="N233" s="3"/>
+      <c r="O233" s="3"/>
+      <c r="P233" s="3"/>
+      <c r="Q233" s="3"/>
+      <c r="R233" s="3"/>
+      <c r="S233" s="3"/>
+      <c r="T233" s="3"/>
+      <c r="U233" s="3"/>
+      <c r="V233" s="9"/>
+    </row>
+    <row r="234" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C234" s="8"/>
+      <c r="D234" s="16"/>
+      <c r="E234" s="3"/>
+      <c r="F234" s="3"/>
+      <c r="G234" s="3"/>
+      <c r="H234" s="3"/>
+      <c r="I234" s="3"/>
+      <c r="J234" s="3"/>
+      <c r="K234" s="3"/>
+      <c r="L234" s="3"/>
+      <c r="M234" s="3"/>
+      <c r="N234" s="3"/>
+      <c r="O234" s="3"/>
+      <c r="P234" s="3"/>
+      <c r="Q234" s="3"/>
+      <c r="R234" s="3"/>
+      <c r="S234" s="3"/>
+      <c r="T234" s="3"/>
+      <c r="U234" s="3"/>
+      <c r="V234" s="9"/>
+    </row>
+    <row r="235" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C235" s="8"/>
+      <c r="D235" s="16"/>
+      <c r="E235" s="3"/>
+      <c r="F235" s="3"/>
+      <c r="G235" s="3"/>
+      <c r="H235" s="3"/>
+      <c r="I235" s="3"/>
+      <c r="J235" s="3"/>
+      <c r="K235" s="3"/>
+      <c r="L235" s="3"/>
+      <c r="M235" s="3"/>
+      <c r="N235" s="3"/>
+      <c r="O235" s="3"/>
+      <c r="P235" s="3"/>
+      <c r="Q235" s="3"/>
+      <c r="R235" s="3"/>
+      <c r="S235" s="3"/>
+      <c r="T235" s="3"/>
+      <c r="U235" s="3"/>
+      <c r="V235" s="9"/>
+    </row>
+    <row r="236" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C236" s="8"/>
+      <c r="D236" s="16"/>
+      <c r="E236" s="3"/>
+      <c r="F236" s="3"/>
+      <c r="G236" s="3"/>
+      <c r="H236" s="3"/>
+      <c r="I236" s="3"/>
+      <c r="J236" s="3"/>
+      <c r="K236" s="3"/>
+      <c r="L236" s="3"/>
+      <c r="M236" s="3"/>
+      <c r="N236" s="3"/>
+      <c r="O236" s="3"/>
+      <c r="P236" s="3"/>
+      <c r="Q236" s="3"/>
+      <c r="R236" s="3"/>
+      <c r="S236" s="3"/>
+      <c r="T236" s="3"/>
+      <c r="U236" s="3"/>
+      <c r="V236" s="9"/>
+    </row>
+    <row r="237" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C237" s="8"/>
+      <c r="D237" s="16"/>
+      <c r="E237" s="3"/>
+      <c r="F237" s="3"/>
+      <c r="G237" s="3"/>
+      <c r="H237" s="3"/>
+      <c r="I237" s="3"/>
+      <c r="J237" s="3"/>
+      <c r="K237" s="3"/>
+      <c r="L237" s="3"/>
+      <c r="M237" s="3"/>
+      <c r="N237" s="3"/>
+      <c r="O237" s="3"/>
+      <c r="P237" s="3"/>
+      <c r="Q237" s="3"/>
+      <c r="R237" s="3"/>
+      <c r="S237" s="3"/>
+      <c r="T237" s="3"/>
+      <c r="U237" s="3"/>
+      <c r="V237" s="9"/>
+    </row>
+    <row r="238" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C238" s="8"/>
+      <c r="D238" s="16"/>
+      <c r="E238" s="3"/>
+      <c r="F238" s="3"/>
+      <c r="G238" s="3"/>
+      <c r="H238" s="3"/>
+      <c r="I238" s="3"/>
+      <c r="J238" s="3"/>
+      <c r="K238" s="3"/>
+      <c r="L238" s="3"/>
+      <c r="M238" s="3"/>
+      <c r="N238" s="3"/>
+      <c r="O238" s="3"/>
+      <c r="P238" s="3"/>
+      <c r="Q238" s="3"/>
+      <c r="R238" s="3"/>
+      <c r="S238" s="3"/>
+      <c r="T238" s="3"/>
+      <c r="U238" s="3"/>
+      <c r="V238" s="9"/>
+    </row>
+    <row r="239" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C239" s="8"/>
+      <c r="D239" s="16"/>
+      <c r="E239" s="3"/>
+      <c r="F239" s="3"/>
+      <c r="G239" s="3"/>
+      <c r="H239" s="3"/>
+      <c r="I239" s="3"/>
+      <c r="J239" s="3"/>
+      <c r="K239" s="3"/>
+      <c r="L239" s="3"/>
+      <c r="M239" s="3"/>
+      <c r="N239" s="3"/>
+      <c r="O239" s="3"/>
+      <c r="P239" s="3"/>
+      <c r="Q239" s="3"/>
+      <c r="R239" s="3"/>
+      <c r="S239" s="3"/>
+      <c r="T239" s="3"/>
+      <c r="U239" s="3"/>
+      <c r="V239" s="9"/>
+    </row>
+    <row r="240" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C240" s="8"/>
+      <c r="D240" s="16"/>
+      <c r="E240" s="3"/>
+      <c r="F240" s="3"/>
+      <c r="G240" s="3"/>
+      <c r="H240" s="3"/>
+      <c r="I240" s="3"/>
+      <c r="J240" s="3"/>
+      <c r="K240" s="3"/>
+      <c r="L240" s="3"/>
+      <c r="M240" s="3"/>
+      <c r="N240" s="3"/>
+      <c r="O240" s="3"/>
+      <c r="P240" s="3"/>
+      <c r="Q240" s="3"/>
+      <c r="R240" s="3"/>
+      <c r="S240" s="3"/>
+      <c r="T240" s="3"/>
+      <c r="U240" s="3"/>
+      <c r="V240" s="9"/>
+    </row>
+    <row r="241" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C241" s="8"/>
+      <c r="D241" s="16"/>
+      <c r="E241" s="3"/>
+      <c r="F241" s="3"/>
+      <c r="G241" s="3"/>
+      <c r="H241" s="3"/>
+      <c r="I241" s="3"/>
+      <c r="J241" s="3"/>
+      <c r="K241" s="3"/>
+      <c r="L241" s="3"/>
+      <c r="M241" s="3"/>
+      <c r="N241" s="3"/>
+      <c r="O241" s="3"/>
+      <c r="P241" s="3"/>
+      <c r="Q241" s="3"/>
+      <c r="R241" s="3"/>
+      <c r="S241" s="3"/>
+      <c r="T241" s="3"/>
+      <c r="U241" s="3"/>
+      <c r="V241" s="9"/>
+    </row>
+    <row r="242" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C242" s="8"/>
+      <c r="D242" s="16"/>
+      <c r="E242" s="3"/>
+      <c r="F242" s="3"/>
+      <c r="G242" s="3"/>
+      <c r="H242" s="3"/>
+      <c r="I242" s="3"/>
+      <c r="J242" s="3"/>
+      <c r="K242" s="3"/>
+      <c r="L242" s="3"/>
+      <c r="M242" s="3"/>
+      <c r="N242" s="3"/>
+      <c r="O242" s="3"/>
+      <c r="P242" s="3"/>
+      <c r="Q242" s="3"/>
+      <c r="R242" s="3"/>
+      <c r="S242" s="3"/>
+      <c r="T242" s="3"/>
+      <c r="U242" s="3"/>
+      <c r="V242" s="9"/>
+    </row>
+    <row r="243" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C243" s="8"/>
+      <c r="D243" s="16"/>
+      <c r="E243" s="3"/>
+      <c r="F243" s="3"/>
+      <c r="G243" s="3"/>
+      <c r="H243" s="3"/>
+      <c r="I243" s="3"/>
+      <c r="J243" s="3"/>
+      <c r="K243" s="3"/>
+      <c r="L243" s="3"/>
+      <c r="M243" s="3"/>
+      <c r="N243" s="3"/>
+      <c r="O243" s="3"/>
+      <c r="P243" s="3"/>
+      <c r="Q243" s="3"/>
+      <c r="R243" s="3"/>
+      <c r="S243" s="3"/>
+      <c r="T243" s="3"/>
+      <c r="U243" s="3"/>
+      <c r="V243" s="9"/>
+    </row>
+    <row r="244" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C244" s="8"/>
+      <c r="D244" s="16"/>
+      <c r="E244" s="3"/>
+      <c r="F244" s="3"/>
+      <c r="G244" s="3"/>
+      <c r="H244" s="3"/>
+      <c r="I244" s="3"/>
+      <c r="J244" s="3"/>
+      <c r="K244" s="3"/>
+      <c r="L244" s="3"/>
+      <c r="M244" s="3"/>
+      <c r="N244" s="3"/>
+      <c r="O244" s="3"/>
+      <c r="P244" s="3"/>
+      <c r="Q244" s="3"/>
+      <c r="R244" s="3"/>
+      <c r="S244" s="3"/>
+      <c r="T244" s="3"/>
+      <c r="U244" s="3"/>
+      <c r="V244" s="9"/>
+    </row>
+    <row r="245" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C245" s="8"/>
+      <c r="D245" s="16"/>
+      <c r="E245" s="3"/>
+      <c r="F245" s="3"/>
+      <c r="G245" s="3"/>
+      <c r="H245" s="3"/>
+      <c r="I245" s="3"/>
+      <c r="J245" s="3"/>
+      <c r="K245" s="3"/>
+      <c r="L245" s="3"/>
+      <c r="M245" s="3"/>
+      <c r="N245" s="3"/>
+      <c r="O245" s="3"/>
+      <c r="P245" s="3"/>
+      <c r="Q245" s="3"/>
+      <c r="R245" s="3"/>
+      <c r="S245" s="3"/>
+      <c r="T245" s="3"/>
+      <c r="U245" s="3"/>
+      <c r="V245" s="9"/>
+    </row>
+    <row r="246" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C246" s="8"/>
+      <c r="D246" s="16"/>
+      <c r="E246" s="3"/>
+      <c r="F246" s="3"/>
+      <c r="G246" s="3"/>
+      <c r="H246" s="3"/>
+      <c r="I246" s="3"/>
+      <c r="J246" s="3"/>
+      <c r="K246" s="3"/>
+      <c r="L246" s="3"/>
+      <c r="M246" s="3"/>
+      <c r="N246" s="3"/>
+      <c r="O246" s="3"/>
+      <c r="P246" s="3"/>
+      <c r="Q246" s="3"/>
+      <c r="R246" s="3"/>
+      <c r="S246" s="3"/>
+      <c r="T246" s="3"/>
+      <c r="U246" s="3"/>
+      <c r="V246" s="9"/>
+    </row>
+    <row r="247" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C247" s="8"/>
+      <c r="D247" s="16"/>
+      <c r="E247" s="3"/>
+      <c r="F247" s="3"/>
+      <c r="G247" s="3"/>
+      <c r="H247" s="3"/>
+      <c r="I247" s="3"/>
+      <c r="J247" s="3"/>
+      <c r="K247" s="3"/>
+      <c r="L247" s="3"/>
+      <c r="M247" s="3"/>
+      <c r="N247" s="3"/>
+      <c r="O247" s="3"/>
+      <c r="P247" s="3"/>
+      <c r="Q247" s="3"/>
+      <c r="R247" s="3"/>
+      <c r="S247" s="3"/>
+      <c r="T247" s="3"/>
+      <c r="U247" s="3"/>
+      <c r="V247" s="9"/>
+    </row>
+    <row r="248" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C248" s="8"/>
+      <c r="D248" s="16"/>
+      <c r="E248" s="3"/>
+      <c r="F248" s="3"/>
+      <c r="G248" s="3"/>
+      <c r="H248" s="3"/>
+      <c r="I248" s="3"/>
+      <c r="J248" s="3"/>
+      <c r="K248" s="3"/>
+      <c r="L248" s="3"/>
+      <c r="M248" s="3"/>
+      <c r="N248" s="3"/>
+      <c r="O248" s="3"/>
+      <c r="P248" s="3"/>
+      <c r="Q248" s="3"/>
+      <c r="R248" s="3"/>
+      <c r="S248" s="3"/>
+      <c r="T248" s="3"/>
+      <c r="U248" s="3"/>
+      <c r="V248" s="9"/>
+    </row>
+    <row r="249" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C249" s="8"/>
+      <c r="D249" s="16"/>
+      <c r="E249" s="3"/>
+      <c r="F249" s="3"/>
+      <c r="G249" s="3"/>
+      <c r="H249" s="3"/>
+      <c r="I249" s="3"/>
+      <c r="J249" s="3"/>
+      <c r="K249" s="3"/>
+      <c r="L249" s="3"/>
+      <c r="M249" s="3"/>
+      <c r="N249" s="3"/>
+      <c r="O249" s="3"/>
+      <c r="P249" s="3"/>
+      <c r="Q249" s="3"/>
+      <c r="R249" s="3"/>
+      <c r="S249" s="3"/>
+      <c r="T249" s="3"/>
+      <c r="U249" s="3"/>
+      <c r="V249" s="9"/>
+    </row>
+    <row r="250" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C250" s="8"/>
+      <c r="D250" s="16"/>
+      <c r="E250" s="3"/>
+      <c r="F250" s="3"/>
+      <c r="G250" s="3"/>
+      <c r="H250" s="3"/>
+      <c r="I250" s="3"/>
+      <c r="J250" s="3"/>
+      <c r="K250" s="3"/>
+      <c r="L250" s="3"/>
+      <c r="M250" s="3"/>
+      <c r="N250" s="3"/>
+      <c r="O250" s="3"/>
+      <c r="P250" s="3"/>
+      <c r="Q250" s="3"/>
+      <c r="R250" s="3"/>
+      <c r="S250" s="3"/>
+      <c r="T250" s="3"/>
+      <c r="U250" s="3"/>
+      <c r="V250" s="9"/>
+    </row>
+    <row r="251" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C251" s="8"/>
+      <c r="D251" s="16"/>
+      <c r="E251" s="3"/>
+      <c r="F251" s="3"/>
+      <c r="G251" s="3"/>
+      <c r="H251" s="3"/>
+      <c r="I251" s="3"/>
+      <c r="J251" s="3"/>
+      <c r="K251" s="3"/>
+      <c r="L251" s="3"/>
+      <c r="M251" s="3"/>
+      <c r="N251" s="3"/>
+      <c r="O251" s="3"/>
+      <c r="P251" s="3"/>
+      <c r="Q251" s="3"/>
+      <c r="R251" s="3"/>
+      <c r="S251" s="3"/>
+      <c r="T251" s="3"/>
+      <c r="U251" s="3"/>
+      <c r="V251" s="9"/>
+    </row>
+    <row r="252" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C252" s="8"/>
+      <c r="D252" s="16"/>
+      <c r="E252" s="3"/>
+      <c r="F252" s="3"/>
+      <c r="G252" s="3"/>
+      <c r="H252" s="3"/>
+      <c r="I252" s="3"/>
+      <c r="J252" s="3"/>
+      <c r="K252" s="3"/>
+      <c r="L252" s="3"/>
+      <c r="M252" s="3"/>
+      <c r="N252" s="3"/>
+      <c r="O252" s="3"/>
+      <c r="P252" s="3"/>
+      <c r="Q252" s="3"/>
+      <c r="R252" s="3"/>
+      <c r="S252" s="3"/>
+      <c r="T252" s="3"/>
+      <c r="U252" s="3"/>
+      <c r="V252" s="9"/>
+    </row>
+    <row r="253" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C253" s="8"/>
+      <c r="D253" s="16"/>
+      <c r="E253" s="3"/>
+      <c r="F253" s="3"/>
+      <c r="G253" s="3"/>
+      <c r="H253" s="3"/>
+      <c r="I253" s="3"/>
+      <c r="J253" s="3"/>
+      <c r="K253" s="3"/>
+      <c r="L253" s="3"/>
+      <c r="M253" s="3"/>
+      <c r="N253" s="3"/>
+      <c r="O253" s="3"/>
+      <c r="P253" s="3"/>
+      <c r="Q253" s="3"/>
+      <c r="R253" s="3"/>
+      <c r="S253" s="3"/>
+      <c r="T253" s="3"/>
+      <c r="U253" s="3"/>
+      <c r="V253" s="9"/>
+    </row>
+    <row r="254" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C254" s="8"/>
+      <c r="D254" s="16"/>
+      <c r="E254" s="3"/>
+      <c r="F254" s="3"/>
+      <c r="G254" s="3"/>
+      <c r="H254" s="3"/>
+      <c r="I254" s="3"/>
+      <c r="J254" s="3"/>
+      <c r="K254" s="3"/>
+      <c r="L254" s="3"/>
+      <c r="M254" s="3"/>
+      <c r="N254" s="3"/>
+      <c r="O254" s="3"/>
+      <c r="P254" s="3"/>
+      <c r="Q254" s="3"/>
+      <c r="R254" s="3"/>
+      <c r="S254" s="3"/>
+      <c r="T254" s="3"/>
+      <c r="U254" s="3"/>
+      <c r="V254" s="9"/>
+    </row>
+    <row r="255" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C255" s="8"/>
+      <c r="D255" s="16"/>
+      <c r="E255" s="3"/>
+      <c r="F255" s="3"/>
+      <c r="G255" s="3"/>
+      <c r="H255" s="3"/>
+      <c r="I255" s="3"/>
+      <c r="J255" s="3"/>
+      <c r="K255" s="3"/>
+      <c r="L255" s="3"/>
+      <c r="M255" s="3"/>
+      <c r="N255" s="3"/>
+      <c r="O255" s="3"/>
+      <c r="P255" s="3"/>
+      <c r="Q255" s="3"/>
+      <c r="R255" s="3"/>
+      <c r="S255" s="3"/>
+      <c r="T255" s="3"/>
+      <c r="U255" s="3"/>
+      <c r="V255" s="9"/>
+    </row>
+    <row r="256" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C256" s="8"/>
+      <c r="D256" s="16"/>
+      <c r="E256" s="3"/>
+      <c r="F256" s="3"/>
+      <c r="G256" s="3"/>
+      <c r="H256" s="3"/>
+      <c r="I256" s="3"/>
+      <c r="J256" s="3"/>
+      <c r="K256" s="3"/>
+      <c r="L256" s="3"/>
+      <c r="M256" s="3"/>
+      <c r="N256" s="3"/>
+      <c r="O256" s="3"/>
+      <c r="P256" s="3"/>
+      <c r="Q256" s="3"/>
+      <c r="R256" s="3"/>
+      <c r="S256" s="3"/>
+      <c r="T256" s="3"/>
+      <c r="U256" s="3"/>
+      <c r="V256" s="9"/>
+    </row>
+    <row r="257" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C257" s="8"/>
+      <c r="D257" s="16"/>
+      <c r="E257" s="3"/>
+      <c r="F257" s="3"/>
+      <c r="G257" s="3"/>
+      <c r="H257" s="3"/>
+      <c r="I257" s="3"/>
+      <c r="J257" s="3"/>
+      <c r="K257" s="3"/>
+      <c r="L257" s="3"/>
+      <c r="M257" s="3"/>
+      <c r="N257" s="3"/>
+      <c r="O257" s="3"/>
+      <c r="P257" s="3"/>
+      <c r="Q257" s="3"/>
+      <c r="R257" s="3"/>
+      <c r="S257" s="3"/>
+      <c r="T257" s="3"/>
+      <c r="U257" s="3"/>
+      <c r="V257" s="9"/>
+    </row>
+    <row r="258" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C258" s="8"/>
+      <c r="D258" s="16"/>
+      <c r="E258" s="3"/>
+      <c r="F258" s="3"/>
+      <c r="G258" s="3"/>
+      <c r="H258" s="3"/>
+      <c r="I258" s="3"/>
+      <c r="J258" s="3"/>
+      <c r="K258" s="3"/>
+      <c r="L258" s="3"/>
+      <c r="M258" s="3"/>
+      <c r="N258" s="3"/>
+      <c r="O258" s="3"/>
+      <c r="P258" s="3"/>
+      <c r="Q258" s="3"/>
+      <c r="R258" s="3"/>
+      <c r="S258" s="3"/>
+      <c r="T258" s="3"/>
+      <c r="U258" s="3"/>
+      <c r="V258" s="9"/>
+    </row>
+    <row r="259" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C259" s="8"/>
+      <c r="D259" s="16"/>
+      <c r="E259" s="3"/>
+      <c r="F259" s="3"/>
+      <c r="G259" s="3"/>
+      <c r="H259" s="3"/>
+      <c r="I259" s="3"/>
+      <c r="J259" s="3"/>
+      <c r="K259" s="3"/>
+      <c r="L259" s="3"/>
+      <c r="M259" s="3"/>
+      <c r="N259" s="3"/>
+      <c r="O259" s="3"/>
+      <c r="P259" s="3"/>
+      <c r="Q259" s="3"/>
+      <c r="R259" s="3"/>
+      <c r="S259" s="3"/>
+      <c r="T259" s="3"/>
+      <c r="U259" s="3"/>
+      <c r="V259" s="9"/>
+    </row>
+    <row r="260" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C260" s="8"/>
+      <c r="D260" s="16"/>
+      <c r="E260" s="3"/>
+      <c r="F260" s="3"/>
+      <c r="G260" s="3"/>
+      <c r="H260" s="3"/>
+      <c r="I260" s="3"/>
+      <c r="J260" s="3"/>
+      <c r="K260" s="3"/>
+      <c r="L260" s="3"/>
+      <c r="M260" s="3"/>
+      <c r="N260" s="3"/>
+      <c r="O260" s="3"/>
+      <c r="P260" s="3"/>
+      <c r="Q260" s="3"/>
+      <c r="R260" s="3"/>
+      <c r="S260" s="3"/>
+      <c r="T260" s="3"/>
+      <c r="U260" s="3"/>
+      <c r="V260" s="9"/>
+    </row>
+    <row r="261" spans="3:22" ht="14.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C261" s="10"/>
+      <c r="D261" s="17"/>
+      <c r="E261" s="11"/>
+      <c r="F261" s="11"/>
+      <c r="G261" s="11"/>
+      <c r="H261" s="11"/>
+      <c r="I261" s="11"/>
+      <c r="J261" s="11"/>
+      <c r="K261" s="11"/>
+      <c r="L261" s="11"/>
+      <c r="M261" s="11"/>
+      <c r="N261" s="11"/>
+      <c r="O261" s="11"/>
+      <c r="P261" s="11"/>
+      <c r="Q261" s="11"/>
+      <c r="R261" s="11"/>
+      <c r="S261" s="11"/>
+      <c r="T261" s="11"/>
+      <c r="U261" s="11"/>
+      <c r="V261" s="12"/>
+    </row>
+    <row r="262" spans="3:22" ht="14.25" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>

</xml_diff>